<commit_message>
updated metadata to round 3 imaging
</commit_message>
<xml_diff>
--- a/paramaters/metadata.xlsx
+++ b/paramaters/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\DELTA_iDISCO\logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moharb/Repos/DELTA_iDISCO/paramaters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F3472E-E0DD-4910-8365-4DEC5D97F4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F7A837-C269-2841-AA75-8E0C453F9A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25248" yWindow="0" windowWidth="20928" windowHeight="25296" xr2:uid="{745E1EB6-071C-45F7-9AB8-2E4ECE02DBF4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{745E1EB6-071C-45F7-9AB8-2E4ECE02DBF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="61">
   <si>
     <t>female</t>
   </si>
@@ -217,13 +217,16 @@
   </si>
   <si>
     <t>CF3</t>
+  </si>
+  <si>
+    <t>/nrs/spruston/Boaz/I2/202410_iDisco_Run3_mousecity/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -638,24 +641,24 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="58.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" customWidth="1"/>
+    <col min="10" max="10" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" customWidth="1"/>
     <col min="12" max="13" width="19.33203125" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -699,7 +702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -744,7 +747,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -789,7 +792,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -834,7 +837,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -879,7 +882,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -924,7 +927,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -969,7 +972,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1059,7 +1062,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1194,7 +1197,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1329,7 +1332,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>45568</v>
       </c>
       <c r="J16" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="K16" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
@@ -1374,18 +1377,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>222638</v>
+        <v>220742</v>
       </c>
       <c r="C17">
-        <v>553920</v>
+        <v>550437</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -1394,43 +1397,43 @@
         <v>6</v>
       </c>
       <c r="G17" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H17" s="1">
-        <v>45425</v>
+        <v>45377</v>
       </c>
       <c r="I17" s="1">
-        <v>45583</v>
+        <v>45554</v>
       </c>
       <c r="J17" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="K17" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
-        <v>5.2666666666666666</v>
+        <v>5.9</v>
       </c>
       <c r="L17">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M17" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="N17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>220678</v>
+        <v>220742</v>
       </c>
       <c r="C18">
-        <v>554459</v>
+        <v>550438</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -1442,29 +1445,29 @@
         <v>9</v>
       </c>
       <c r="H18" s="1">
-        <v>45430</v>
+        <v>45377</v>
       </c>
       <c r="I18" s="1">
-        <v>45583</v>
+        <v>45554</v>
       </c>
       <c r="J18" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="K18" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
-        <v>5.0999999999999996</v>
+        <v>5.9</v>
       </c>
       <c r="L18">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M18" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="N18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>220742</v>
       </c>
       <c r="C19">
-        <v>550437</v>
+        <v>550439</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -1493,7 +1496,7 @@
         <v>45554</v>
       </c>
       <c r="J19" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="K19" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
@@ -1506,18 +1509,18 @@
         <v>52</v>
       </c>
       <c r="N19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>220742</v>
+        <v>220743</v>
       </c>
       <c r="C20">
-        <v>550438</v>
+        <v>551775</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -1532,17 +1535,17 @@
         <v>9</v>
       </c>
       <c r="H20" s="1">
-        <v>45377</v>
+        <v>45393</v>
       </c>
       <c r="I20" s="1">
         <v>45554</v>
       </c>
       <c r="J20" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="K20" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
-        <v>5.9</v>
+        <v>5.3666666666666663</v>
       </c>
       <c r="L20">
         <v>8</v>
@@ -1551,18 +1554,18 @@
         <v>52</v>
       </c>
       <c r="N20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>220742</v>
+        <v>220743</v>
       </c>
       <c r="C21">
-        <v>550439</v>
+        <v>551775</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
@@ -1577,17 +1580,17 @@
         <v>9</v>
       </c>
       <c r="H21" s="1">
-        <v>45377</v>
+        <v>45393</v>
       </c>
       <c r="I21" s="1">
         <v>45554</v>
       </c>
       <c r="J21" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="K21" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
-        <v>5.9</v>
+        <v>5.3666666666666663</v>
       </c>
       <c r="L21">
         <v>8</v>
@@ -1596,10 +1599,10 @@
         <v>52</v>
       </c>
       <c r="N21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>45554</v>
       </c>
       <c r="J22" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="K22" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
@@ -1641,21 +1644,21 @@
         <v>52</v>
       </c>
       <c r="N22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>220743</v>
+        <v>222638</v>
       </c>
       <c r="C23">
-        <v>551775</v>
+        <v>553920</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
@@ -1664,43 +1667,43 @@
         <v>6</v>
       </c>
       <c r="G23" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>45393</v>
+        <v>45425</v>
       </c>
       <c r="I23" s="1">
-        <v>45554</v>
+        <v>45583</v>
       </c>
       <c r="J23" t="s">
         <v>43</v>
       </c>
       <c r="K23" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
-        <v>5.3666666666666663</v>
+        <v>5.2666666666666666</v>
       </c>
       <c r="L23">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M23" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="N23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>220743</v>
+        <v>220678</v>
       </c>
       <c r="C24">
-        <v>551775</v>
+        <v>554459</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
@@ -1712,29 +1715,29 @@
         <v>9</v>
       </c>
       <c r="H24" s="1">
-        <v>45393</v>
+        <v>45430</v>
       </c>
       <c r="I24" s="1">
-        <v>45554</v>
+        <v>45583</v>
       </c>
       <c r="J24" t="s">
         <v>43</v>
       </c>
       <c r="K24" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
-        <v>5.3666666666666663</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="L24">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M24" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="N24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1779,7 +1782,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1824,7 +1827,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1869,7 +1872,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1914,7 +1917,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1959,7 +1962,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2059,12 +2062,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2078,7 +2081,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2092,7 +2095,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2106,7 +2109,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
@@ -2117,7 +2120,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>14</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>15</v>
       </c>
@@ -2133,12 +2136,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
error in metadata mouscity numbers
</commit_message>
<xml_diff>
--- a/paramaters/metadata.xlsx
+++ b/paramaters/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moharb/Repos/DELTA_iDISCO/paramaters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\DELTA_iDISCO\paramaters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F7A837-C269-2841-AA75-8E0C453F9A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4BA049-9DEC-45EC-BBFF-7BD169D585AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{745E1EB6-071C-45F7-9AB8-2E4ECE02DBF4}"/>
+    <workbookView xWindow="3552" yWindow="3120" windowWidth="19464" windowHeight="11232" xr2:uid="{745E1EB6-071C-45F7-9AB8-2E4ECE02DBF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -226,7 +226,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -640,25 +640,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{683598A3-2D17-4BD1-A232-F944C044D30F}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E21" activeCellId="1" sqref="C23 E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="58.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="58.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" customWidth="1"/>
     <col min="12" max="13" width="19.33203125" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -702,7 +702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>1</v>
       </c>
@@ -747,7 +747,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>2</v>
       </c>
@@ -792,7 +792,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>3</v>
       </c>
@@ -837,7 +837,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>4</v>
       </c>
@@ -882,7 +882,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>5</v>
       </c>
@@ -927,7 +927,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7">
         <v>6</v>
       </c>
@@ -972,7 +972,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>220743</v>
       </c>
       <c r="C21">
-        <v>551775</v>
+        <v>551776</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
@@ -1602,7 +1602,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>220743</v>
       </c>
       <c r="C22">
-        <v>551775</v>
+        <v>551777</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
@@ -1647,7 +1647,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2062,12 +2062,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="C5" t="s">
         <v>14</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="C6" t="s">
         <v>15</v>
       </c>
@@ -2136,12 +2136,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="D7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="D8" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Update on reversal and metadata with shortName
</commit_message>
<xml_diff>
--- a/paramaters/metadata.xlsx
+++ b/paramaters/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\DELTA_iDISCO\paramaters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4486072A-8188-44D2-A355-F6187971A42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0158BF0-6776-4C0C-8E9F-58D27EA15903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{745E1EB6-071C-45F7-9AB8-2E4ECE02DBF4}"/>
   </bookViews>
@@ -675,7 +675,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -686,10 +686,12 @@
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="58.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" customWidth="1"/>
     <col min="11" max="11" width="9.109375" customWidth="1"/>
-    <col min="12" max="14" width="19.33203125" customWidth="1"/>
-    <col min="15" max="15" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">

</xml_diff>

<commit_message>
Updated metadata with DOI + MouseCity Round 3
</commit_message>
<xml_diff>
--- a/paramaters/metadata.xlsx
+++ b/paramaters/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moharb/Repos/DELTA_iDISCO/paramaters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moharb/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56010FDD-6A81-214E-8FA5-DAF3CADDA708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8149967-332A-9F43-BBF8-4DFAA5B604EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{745E1EB6-071C-45F7-9AB8-2E4ECE02DBF4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="16780" windowHeight="20140" xr2:uid="{745E1EB6-071C-45F7-9AB8-2E4ECE02DBF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="88">
   <si>
     <t>female</t>
   </si>
@@ -255,7 +255,7 @@
     <t>Z673_5</t>
   </si>
   <si>
-    <t>/nrs/spruston/Boaz/I2/20251001_DOI/</t>
+    <t>/nrs/spruston/Boaz/I2/20250110_IDISCO_DOI</t>
   </si>
   <si>
     <t>DOI</t>
@@ -282,7 +282,7 @@
     <t>DMSO3</t>
   </si>
   <si>
-    <t>/nrs/spruston/Boaz/I2/20251001_MouseCity3/</t>
+    <t>/nrs/spruston/Boaz/I2/20250111_IDISCO_MouseCity3</t>
   </si>
   <si>
     <t>MC3_A</t>
@@ -301,9 +301,6 @@
   </si>
   <si>
     <t>MC3_F</t>
-  </si>
-  <si>
-    <t>Might be issue in cortex/</t>
   </si>
 </sst>
 </file>
@@ -725,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{683598A3-2D17-4BD1-A232-F944C044D30F}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2192,9 +2189,6 @@
       <c r="N32" t="s">
         <v>76</v>
       </c>
-      <c r="O32" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -2381,10 +2375,10 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>220742</v>
+        <v>223896</v>
       </c>
       <c r="C37">
-        <v>550437</v>
+        <v>556543</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
@@ -2399,20 +2393,20 @@
         <v>9</v>
       </c>
       <c r="H37" s="1">
-        <v>45377</v>
+        <v>45459</v>
       </c>
       <c r="I37" s="1">
-        <v>45554</v>
+        <v>45630</v>
       </c>
       <c r="J37" t="s">
         <v>81</v>
       </c>
       <c r="K37" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
-        <v>5.9</v>
+        <v>5.7</v>
       </c>
       <c r="L37">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M37" t="s">
         <v>50</v>
@@ -2426,10 +2420,10 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>220742</v>
+        <v>223896</v>
       </c>
       <c r="C38">
-        <v>550438</v>
+        <v>556544</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
@@ -2444,20 +2438,20 @@
         <v>9</v>
       </c>
       <c r="H38" s="1">
-        <v>45377</v>
+        <v>45459</v>
       </c>
       <c r="I38" s="1">
-        <v>45554</v>
+        <v>45630</v>
       </c>
       <c r="J38" t="s">
         <v>81</v>
       </c>
       <c r="K38" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
-        <v>5.9</v>
+        <v>5.7</v>
       </c>
       <c r="L38">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M38" t="s">
         <v>50</v>
@@ -2471,10 +2465,10 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>220742</v>
+        <v>223896</v>
       </c>
       <c r="C39">
-        <v>550439</v>
+        <v>556545</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
@@ -2489,20 +2483,20 @@
         <v>9</v>
       </c>
       <c r="H39" s="1">
-        <v>45377</v>
+        <v>45459</v>
       </c>
       <c r="I39" s="1">
-        <v>45554</v>
+        <v>45630</v>
       </c>
       <c r="J39" t="s">
         <v>81</v>
       </c>
       <c r="K39" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
-        <v>5.9</v>
+        <v>5.7</v>
       </c>
       <c r="L39">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M39" t="s">
         <v>50</v>
@@ -2516,10 +2510,10 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>220743</v>
+        <v>218788</v>
       </c>
       <c r="C40">
-        <v>551775</v>
+        <v>555974</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -2534,20 +2528,20 @@
         <v>9</v>
       </c>
       <c r="H40" s="1">
-        <v>45393</v>
+        <v>45450</v>
       </c>
       <c r="I40" s="1">
-        <v>45554</v>
+        <v>45630</v>
       </c>
       <c r="J40" t="s">
         <v>81</v>
       </c>
       <c r="K40" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
-        <v>5.3666666666666663</v>
+        <v>6</v>
       </c>
       <c r="L40">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M40" t="s">
         <v>50</v>
@@ -2561,10 +2555,10 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>220743</v>
+        <v>218788</v>
       </c>
       <c r="C41">
-        <v>551776</v>
+        <v>555975</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -2579,20 +2573,20 @@
         <v>9</v>
       </c>
       <c r="H41" s="1">
-        <v>45393</v>
+        <v>45450</v>
       </c>
       <c r="I41" s="1">
-        <v>45554</v>
+        <v>45630</v>
       </c>
       <c r="J41" t="s">
         <v>81</v>
       </c>
       <c r="K41" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
-        <v>5.3666666666666663</v>
+        <v>6</v>
       </c>
       <c r="L41">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M41" t="s">
         <v>50</v>
@@ -2606,10 +2600,10 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>220743</v>
+        <v>218788</v>
       </c>
       <c r="C42">
-        <v>551777</v>
+        <v>555976</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -2624,20 +2618,20 @@
         <v>9</v>
       </c>
       <c r="H42" s="1">
-        <v>45393</v>
+        <v>45450</v>
       </c>
       <c r="I42" s="1">
-        <v>45554</v>
+        <v>45630</v>
       </c>
       <c r="J42" t="s">
         <v>81</v>
       </c>
       <c r="K42" s="3">
         <f>IF(_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30&gt;0,_xlfn.DAYS(Table1[[#This Row],[Perfusion]],Table1[[#This Row],[DOB]])/30,0)</f>
-        <v>5.3666666666666663</v>
+        <v>6</v>
       </c>
       <c r="L42">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M42" t="s">
         <v>50</v>
@@ -2653,7 +2647,7 @@
       <formula1>100000</formula1>
       <formula2>999999</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H30" xr:uid="{D7AA6B52-0D0A-4557-8F73-2BE98376B947}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H42" xr:uid="{D7AA6B52-0D0A-4557-8F73-2BE98376B947}">
       <formula1>43831</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>